<commit_message>
Updated for dates 1st and 3rd April
</commit_message>
<xml_diff>
--- a/Daily Status update Report.xlsx
+++ b/Daily Status update Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,8 @@
     <sheet name="27-Mar" sheetId="7" r:id="rId7"/>
     <sheet name="30-Mar" sheetId="8" r:id="rId8"/>
     <sheet name="31-Mar" sheetId="9" r:id="rId9"/>
+    <sheet name="1-Apr" sheetId="10" r:id="rId10"/>
+    <sheet name="3-Apr" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="100">
   <si>
     <t>Employee Name</t>
   </si>
@@ -332,8 +334,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,21 +753,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -776,7 +778,7 @@
     <col min="7" max="7" width="117.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -799,7 +801,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -822,7 +824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -845,7 +847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -868,7 +870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -891,7 +893,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -914,7 +916,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -937,7 +939,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -960,7 +962,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -983,7 +985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1006,7 +1008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1029,7 +1031,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1050,7 +1052,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1077,15 +1079,527 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="25">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="26">
+        <v>13</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G14" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="25">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="26">
+        <v>13</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G14" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1096,7 +1610,7 @@
     <col min="7" max="7" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1119,7 +1633,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1142,7 +1656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1165,7 +1679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1188,7 +1702,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1211,7 +1725,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1234,7 +1748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1257,7 +1771,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1280,7 +1794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1303,7 +1817,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1326,7 +1840,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1349,7 +1863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1372,7 +1886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1402,14 +1916,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1420,7 +1934,7 @@
     <col min="7" max="7" width="136.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1443,7 +1957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1466,7 +1980,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1489,7 +2003,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1512,7 +2026,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1535,7 +2049,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1558,7 +2072,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1581,7 +2095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1604,7 +2118,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1627,7 +2141,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -1650,7 +2164,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1673,7 +2187,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -1696,7 +2210,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -1726,14 +2240,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1744,7 +2258,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1767,7 +2281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1790,7 +2304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1813,7 +2327,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1836,7 +2350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1859,7 +2373,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1882,7 +2396,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1905,7 +2419,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1928,7 +2442,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1951,7 +2465,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -1974,7 +2488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1997,7 +2511,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2020,7 +2534,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2043,7 +2557,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2073,14 +2587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -2091,7 +2605,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2114,7 +2628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2137,7 +2651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2160,7 +2674,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2183,7 +2697,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2206,7 +2720,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2229,7 +2743,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2252,7 +2766,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2275,7 +2789,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2298,7 +2812,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2321,7 +2835,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2344,7 +2858,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2367,7 +2881,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2390,7 +2904,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2420,14 +2934,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -2438,7 +2952,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2461,7 +2975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2484,7 +2998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2507,7 +3021,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2530,7 +3044,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2553,7 +3067,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2576,7 +3090,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2599,7 +3113,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2622,7 +3136,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2645,7 +3159,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2668,7 +3182,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2691,7 +3205,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2714,7 +3228,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2737,7 +3251,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2767,14 +3281,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -2785,7 +3299,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2808,7 +3322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2831,7 +3345,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2854,7 +3368,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2877,7 +3391,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2900,7 +3414,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2923,7 +3437,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2946,7 +3460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2969,7 +3483,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2992,7 +3506,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3015,7 +3529,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3038,7 +3552,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3061,7 +3575,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3084,7 +3598,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3114,14 +3628,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -3132,7 +3646,7 @@
     <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
@@ -3155,7 +3669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3178,7 +3692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -3201,7 +3715,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -3224,7 +3738,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -3247,7 +3761,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -3270,7 +3784,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -3293,7 +3807,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -3316,7 +3830,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -3339,7 +3853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -3362,7 +3876,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -3385,7 +3899,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -3408,7 +3922,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -3431,7 +3945,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -3461,14 +3975,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3479,7 +3993,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3502,7 +4016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3515,7 +4029,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3528,7 +4042,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3541,7 +4055,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3554,7 +4068,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3567,7 +4081,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3580,7 +4094,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3593,7 +4107,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3606,7 +4120,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -3629,7 +4143,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -3652,7 +4166,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -3675,7 +4189,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -3698,7 +4212,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Updated for date 1st April
</commit_message>
<xml_diff>
--- a/Daily Status update Report.xlsx
+++ b/Daily Status update Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="31-Mar" sheetId="9" r:id="rId9"/>
     <sheet name="1-Apr" sheetId="10" r:id="rId10"/>
     <sheet name="3-Apr" sheetId="11" r:id="rId11"/>
+    <sheet name="7-Apr" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="102">
   <si>
     <t>Employee Name</t>
   </si>
@@ -329,13 +330,19 @@
   </si>
   <si>
     <t>Updating test cases for API Testing - Collateral flow (Deposit Cash - Unchecked /checked scenario)-Manually Settled and Manually Rejected</t>
+  </si>
+  <si>
+    <t>Updated Test cases for API Testing- Collateral flow(Unchecked-Unchecked &amp; Checked-Unchecked Scenarios)</t>
+  </si>
+  <si>
+    <t>Going through SLA document;Git setup; Cucumber set up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +362,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -403,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -481,6 +494,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,7 +767,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1246,7 +1260,7 @@
       </c>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="16.5">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -1265,7 +1279,9 @@
       <c r="F11" s="28">
         <v>0.75</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="29" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="25">
@@ -1286,7 +1302,9 @@
       <c r="F12" s="28">
         <v>0.75</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="25" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="25">
@@ -1332,6 +1350,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1339,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="A1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1391,6 +1410,262 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="25">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="26">
+        <v>13</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G14" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3285,7 +3560,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3525,7 +3800,7 @@
       <c r="F10" s="19">
         <v>0.75</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="25" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3979,7 +4254,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated for 4 th apr
</commit_message>
<xml_diff>
--- a/Daily Status update Report.xlsx
+++ b/Daily Status update Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="31-Mar" sheetId="9" r:id="rId9"/>
     <sheet name="1-Apr" sheetId="10" r:id="rId10"/>
     <sheet name="3-Apr" sheetId="11" r:id="rId11"/>
+    <sheet name="4-Apr" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="100">
   <si>
     <t>Employee Name</t>
   </si>
@@ -334,8 +335,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,21 +754,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -778,7 +779,7 @@
     <col min="7" max="7" width="117.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -801,7 +802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -824,7 +825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -847,7 +848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -870,7 +871,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -893,7 +894,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -916,7 +917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -939,7 +940,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -962,7 +963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -985,7 +986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1008,7 +1009,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1052,7 +1053,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1080,14 +1081,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1098,7 +1099,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1121,7 +1122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1134,7 +1135,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1147,7 +1148,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1160,7 +1161,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1173,7 +1174,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1186,7 +1187,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1199,7 +1200,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1212,7 +1213,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1225,7 +1226,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -1246,7 +1247,7 @@
       </c>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -1267,7 +1268,7 @@
       </c>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -1288,7 +1289,7 @@
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -1309,7 +1310,7 @@
       </c>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -1336,14 +1337,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1354,7 +1355,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1390,7 +1391,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1403,7 +1404,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1416,7 +1417,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1429,7 +1430,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1442,7 +1443,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1455,7 +1456,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1468,7 +1469,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1481,7 +1482,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -1502,7 +1503,7 @@
       </c>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -1523,7 +1524,7 @@
       </c>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -1544,7 +1545,7 @@
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -1565,7 +1566,263 @@
       </c>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>13</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="28">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F14" s="28">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G14" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="27">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="25">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -1592,14 +1849,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1610,7 +1867,7 @@
     <col min="7" max="7" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1633,7 +1890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1656,7 +1913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1679,7 +1936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1702,7 +1959,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1725,7 +1982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1748,7 +2005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1771,7 +2028,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1794,7 +2051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1817,7 +2074,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1840,7 +2097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1863,7 +2120,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1886,7 +2143,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1916,14 +2173,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1934,7 +2191,7 @@
     <col min="7" max="7" width="136.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1957,7 +2214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1980,7 +2237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2003,7 +2260,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2026,7 +2283,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2049,7 +2306,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2072,7 +2329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2095,7 +2352,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2118,7 +2375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2141,7 +2398,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2164,7 +2421,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2187,7 +2444,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2210,7 +2467,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2240,14 +2497,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2258,7 +2515,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2281,7 +2538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2304,7 +2561,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2327,7 +2584,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2350,7 +2607,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2373,7 +2630,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2396,7 +2653,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2419,7 +2676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2442,7 +2699,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2465,7 +2722,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2488,7 +2745,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2511,7 +2768,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2534,7 +2791,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2557,7 +2814,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2587,14 +2844,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -2605,7 +2862,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2628,7 +2885,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2651,7 +2908,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2674,7 +2931,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2697,7 +2954,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2720,7 +2977,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2743,7 +3000,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2766,7 +3023,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2789,7 +3046,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2812,7 +3069,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2835,7 +3092,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2858,7 +3115,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2881,7 +3138,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2904,7 +3161,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2934,14 +3191,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -2952,7 +3209,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2975,7 +3232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2998,7 +3255,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3021,7 +3278,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3044,7 +3301,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3067,7 +3324,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3090,7 +3347,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3113,7 +3370,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3136,7 +3393,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3159,7 +3416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3182,7 +3439,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3205,7 +3462,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3228,7 +3485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3251,7 +3508,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3281,14 +3538,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3299,7 +3556,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3322,7 +3579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3345,7 +3602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3368,7 +3625,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3391,7 +3648,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3414,7 +3671,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3437,7 +3694,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3460,7 +3717,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3483,7 +3740,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3506,7 +3763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3529,7 +3786,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3552,7 +3809,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3575,7 +3832,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3598,7 +3855,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3628,14 +3885,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -3646,7 +3903,7 @@
     <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
@@ -3669,7 +3926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3692,7 +3949,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -3715,7 +3972,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -3738,7 +3995,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -3761,7 +4018,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -3784,7 +4041,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -3807,7 +4064,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -3830,7 +4087,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -3853,7 +4110,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -3876,7 +4133,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -3899,7 +4156,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -3922,7 +4179,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -3945,7 +4202,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -3975,14 +4232,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3993,7 +4250,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4016,7 +4273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4029,7 +4286,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4042,7 +4299,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4055,7 +4312,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4068,7 +4325,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4081,7 +4338,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4094,7 +4351,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4107,7 +4364,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4120,7 +4377,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -4143,7 +4400,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -4166,7 +4423,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -4189,7 +4446,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -4212,7 +4469,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Status Updated for 1st April 2020
</commit_message>
<xml_diff>
--- a/Daily Status update Report.xlsx
+++ b/Daily Status update Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6855" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="19-Mar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="3-Apr" sheetId="11" r:id="rId11"/>
     <sheet name="4-Apr" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="101">
   <si>
     <t>Employee Name</t>
   </si>
@@ -330,13 +330,16 @@
   </si>
   <si>
     <t>Updating test cases for API Testing - Collateral flow (Deposit Cash - Unchecked /checked scenario)-Manually Settled and Manually Rejected</t>
+  </si>
+  <si>
+    <t>Understanding Git Bash</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,21 +757,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -779,7 +782,7 @@
     <col min="7" max="7" width="117.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -802,7 +805,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -825,7 +828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -848,7 +851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -871,7 +874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -894,7 +897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -917,7 +920,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -940,7 +943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -963,7 +966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -986,7 +989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1053,7 +1056,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1081,14 +1084,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1099,7 +1102,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1135,7 +1138,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1148,7 +1151,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1161,7 +1164,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1174,7 +1177,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1187,7 +1190,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1200,7 +1203,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1213,7 +1216,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1226,7 +1229,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -1247,7 +1250,7 @@
       </c>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -1268,7 +1271,7 @@
       </c>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -1289,7 +1292,7 @@
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -1303,14 +1306,16 @@
         <v>15</v>
       </c>
       <c r="E13" s="27">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F13" s="28">
         <v>0.75</v>
       </c>
-      <c r="G13" s="25"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -1337,14 +1342,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1355,7 +1360,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1378,7 +1383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1391,7 +1396,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1404,7 +1409,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1417,7 +1422,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1430,7 +1435,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1443,7 +1448,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1456,7 +1461,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1469,7 +1474,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1482,7 +1487,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -1503,7 +1508,7 @@
       </c>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -1524,7 +1529,7 @@
       </c>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -1545,7 +1550,7 @@
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -1566,7 +1571,7 @@
       </c>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -1593,14 +1598,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1611,7 +1616,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1634,7 +1639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1647,7 +1652,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1660,7 +1665,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1673,7 +1678,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1686,7 +1691,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1699,7 +1704,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1712,7 +1717,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1725,7 +1730,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1738,7 +1743,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -1759,7 +1764,7 @@
       </c>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -1780,7 +1785,7 @@
       </c>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -1801,7 +1806,7 @@
       </c>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -1822,7 +1827,7 @@
       </c>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -1849,14 +1854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -1867,7 +1872,7 @@
     <col min="7" max="7" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1890,7 +1895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1913,7 +1918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1936,7 +1941,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1959,7 +1964,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1982,7 +1987,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2005,7 +2010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2028,7 +2033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2051,7 +2056,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2074,7 +2079,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2097,7 +2102,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2120,7 +2125,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2143,7 +2148,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2173,14 +2178,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2191,7 +2196,7 @@
     <col min="7" max="7" width="136.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2214,7 +2219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2237,7 +2242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2260,7 +2265,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2283,7 +2288,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2306,7 +2311,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2329,7 +2334,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2352,7 +2357,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2375,7 +2380,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2398,7 +2403,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2421,7 +2426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2444,7 +2449,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2467,7 +2472,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2497,14 +2502,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -2515,7 +2520,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2538,7 +2543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2561,7 +2566,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2584,7 +2589,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2607,7 +2612,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2630,7 +2635,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2653,7 +2658,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2676,7 +2681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2699,7 +2704,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2722,7 +2727,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2745,7 +2750,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2768,7 +2773,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2791,7 +2796,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2814,7 +2819,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2844,14 +2849,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -2862,7 +2867,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2885,7 +2890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2908,7 +2913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2931,7 +2936,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2977,7 +2982,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3000,7 +3005,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3023,7 +3028,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3046,7 +3051,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3069,7 +3074,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3092,7 +3097,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3115,7 +3120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3138,7 +3143,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3161,7 +3166,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3191,14 +3196,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3209,7 +3214,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3232,7 +3237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3255,7 +3260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3278,7 +3283,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3301,7 +3306,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3324,7 +3329,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3347,7 +3352,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3393,7 +3398,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3416,7 +3421,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3439,7 +3444,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3462,7 +3467,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3485,7 +3490,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3508,7 +3513,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3538,14 +3543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3556,7 +3561,7 @@
     <col min="7" max="7" width="134.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3579,7 +3584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3602,7 +3607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3625,7 +3630,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3648,7 +3653,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3671,7 +3676,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3694,7 +3699,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3717,7 +3722,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3740,7 +3745,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3763,7 +3768,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -3786,7 +3791,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -3809,7 +3814,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -3832,7 +3837,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -3855,7 +3860,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3885,14 +3890,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -3903,7 +3908,7 @@
     <col min="7" max="7" width="99.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
@@ -3926,7 +3931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -3949,7 +3954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -3972,7 +3977,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -3995,7 +4000,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -4018,7 +4023,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -4041,7 +4046,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="22">
         <v>6</v>
       </c>
@@ -4064,7 +4069,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="22">
         <v>7</v>
       </c>
@@ -4087,7 +4092,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="22">
         <v>8</v>
       </c>
@@ -4110,7 +4115,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -4133,7 +4138,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -4156,7 +4161,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -4179,7 +4184,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -4202,7 +4207,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -4232,14 +4237,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -4250,7 +4255,7 @@
     <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4273,7 +4278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4286,7 +4291,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4299,7 +4304,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4312,7 +4317,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -4325,7 +4330,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -4338,7 +4343,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -4351,7 +4356,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -4364,7 +4369,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -4377,7 +4382,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="25">
         <v>9</v>
       </c>
@@ -4400,7 +4405,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="25">
         <v>10</v>
       </c>
@@ -4423,7 +4428,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="25">
         <v>11</v>
       </c>
@@ -4446,7 +4451,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="25">
         <v>12</v>
       </c>
@@ -4469,7 +4474,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="26">
         <v>13</v>
       </c>

</xml_diff>